<commit_message>
Testing Doc Files added
</commit_message>
<xml_diff>
--- a/4.MONITORING AND CONTROLLING PHASE/Testing and Evaluating/Trader PHP/TRADER PHP TESTING.xlsx
+++ b/4.MONITORING AND CONTROLLING PHASE/Testing and Evaluating/Trader PHP/TRADER PHP TESTING.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flex\Desktop\Team-Portfolio\4.MONITORING AND CONTROLLING PHASE\Testing and Evaluating\Trader PHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Portfolio Team Project\Team-Portfolio\4.MONITORING AND CONTROLLING PHASE\Testing and Evaluating\Trader PHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5CFDCD-9FFE-4CB6-AB42-1659E397D206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -192,9 +191,6 @@
     <t>Trader enters an email address which is already used by existing trader</t>
   </si>
   <si>
-    <t xml:space="preserve">Trader inputs password that is less than 8 characters </t>
-  </si>
-  <si>
     <t>Trader inputs password with no uppercase letter, a number or a special character</t>
   </si>
   <si>
@@ -280,12 +276,15 @@
   </si>
   <si>
     <t>Trader is redirected to login page where the trader has to enter their username/email and password</t>
+  </si>
+  <si>
+    <t>Trader inputs password that is less than 8 characters or greater than 32 characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -648,11 +647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -704,7 +703,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -715,10 +714,10 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -732,7 +731,7 @@
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -760,7 +759,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -774,7 +773,7 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -785,10 +784,10 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -799,10 +798,10 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -810,13 +809,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
         <v>81</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>83</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -827,10 +826,10 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -916,7 +915,7 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
@@ -932,10 +931,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -946,10 +945,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -960,10 +959,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -988,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -1002,10 +1001,10 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -1016,10 +1015,10 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
         <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>76</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -1040,10 +1039,10 @@
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -1059,10 +1058,10 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
         <v>64</v>
-      </c>
-      <c r="C41" t="s">
-        <v>65</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>

</xml_diff>